<commit_message>
ok pre final code
</commit_message>
<xml_diff>
--- a/public/sampleCustomers.xlsx
+++ b/public/sampleCustomers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GNG\Desktop\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReactJS\vansale\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Sr.</t>
   </si>
@@ -87,13 +87,16 @@
   </si>
   <si>
     <t>ali123@ali.com</t>
+  </si>
+  <si>
+    <t>Note:All fields are required for every item.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +108,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,10 +142,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A11" sqref="A11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +544,18 @@
         <v>14</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:D11"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
@@ -539,5 +564,6 @@
     <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>